<commit_message>
Updated. CF didn't give any entries so needs retesting. Should add Quikr?
</commit_message>
<xml_diff>
--- a/Automated House Leads.xlsx
+++ b/Automated House Leads.xlsx
@@ -5,19 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="QueryURLs" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="99AcresFilters" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="CommonFloorFilters" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="NoBrokerFilters" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="MagicBricksFilters" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="99Acres" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="CommonFloor" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="NoBroker" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="MagicBricks" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="NoBrokerFilters" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="MagicBricksFilters" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="99Acres" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="NoBroker" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="MagicBricks" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="114">
   <si>
     <t xml:space="preserve">Theory</t>
   </si>
@@ -38,7 +36,8 @@
   </si>
   <si>
     <t xml:space="preserve">URLs usually carry the first set of filters you put when you ran the search. Any additional filters you've added from the search results page are unlikely to reflect here. 
-If you read the part after the .com then you should be able to make out each of the individual conditions - "something field = some value &amp;" or some similar pattern will repeat. The &amp; is just to differentiate one criterion from another.</t>
+If you read the part after the .com then you should be able to make out each of the individual conditions - "something field = some value &amp;" or some similar pattern will repeat. The &amp; is just to differentiate one criterion from another.
+Whatever you aren’t able to capture, you can try and capture in the Filters sheet for the respective website.</t>
   </si>
   <si>
     <t xml:space="preserve">It’s mostly the name of the location which will change across different URLs from the same website. You can try and reuse the rest of the search string as is from a previous URL that you’ve been looking at.</t>
@@ -185,15 +184,6 @@
     <t xml:space="preserve">Need 3 bedrooms</t>
   </si>
   <si>
-    <t xml:space="preserve">contact_person_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">furnish_state</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fully</t>
-  </si>
-  <si>
     <t xml:space="preserve">bathroom</t>
   </si>
   <si>
@@ -215,9 +205,6 @@
     <t xml:space="preserve">Furnishedstatus</t>
   </si>
   <si>
-    <t xml:space="preserve">Furnished</t>
-  </si>
-  <si>
     <t xml:space="preserve">Address</t>
   </si>
   <si>
@@ -248,172 +235,58 @@
     <t xml:space="preserve">ZZStatus</t>
   </si>
   <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">title</t>
+    <t xml:space="preserve">buildingName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaseType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">propertySize</t>
   </si>
   <si>
     <t xml:space="preserve">type</t>
   </si>
   <si>
-    <t xml:space="preserve">bed_rooms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bath_rooms</t>
+    <t xml:space="preserve">locality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">society</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swimmingPool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gym</t>
+  </si>
+  <si>
+    <t xml:space="preserve">furnishing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amenities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">powerBackup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waterSupply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deposit</t>
   </si>
   <si>
     <t xml:space="preserve">balconies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_carpet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_builtup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_unit_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expected_amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deposit_amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">possession_from</t>
-  </si>
-  <si>
-    <t xml:space="preserve">property_age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bachelors_allowed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tenant_veg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">two_wheeler_parking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">four_wheeler_parking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total_floors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">on_floor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">block</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">added_on</t>
-  </si>
-  <si>
-    <t xml:space="preserve">state</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description_by_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">about_project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">car_parking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">location_url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact_person_profile_url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Community.Amenities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green.Living</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Others</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project_url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health...Fitness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kid.Friendly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connectivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZZCallStatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buildingName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">leaseType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">propertySize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">locality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">society</t>
-  </si>
-  <si>
-    <t xml:space="preserve">swimmingPool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gym</t>
-  </si>
-  <si>
-    <t xml:space="preserve">furnishing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">amenities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">powerBackup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waterSupply</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deposit</t>
   </si>
   <si>
     <t xml:space="preserve">lastUpdateDate</t>
@@ -651,15 +524,15 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.64285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.9030612244898"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="14.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,7 +544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="92.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="100.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
@@ -769,144 +642,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AJ1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.9030612244898"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -921,16 +657,16 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="112.852040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="41.0357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="14.9030612244898"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="112.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="41.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="14.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -998,7 +734,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1013,13 +749,13 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.9030612244898"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,7 +841,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1118,15 +854,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.9030612244898"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1149,50 +885,31 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
+      <c r="F2" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1205,15 +922,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F65536"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.9030612244898"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1236,31 +953,50 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1273,81 +1009,62 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.9030612244898"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>44</v>
+        <v>61</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1360,62 +1077,98 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.9030612244898"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="W1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1428,265 +1181,131 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AT1"/>
+  <dimension ref="A1:AJ1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.9030612244898"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>77</v>
+        <v>92</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="AF1" s="3" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="AG1" s="3" t="s">
-        <v>101</v>
+        <v>63</v>
       </c>
       <c r="AH1" s="3" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="AI1" s="3" t="s">
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="AJ1" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="AN1" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="AP1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AR1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AS1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AT1" s="3" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:Y1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.9030612244898"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Keeping backup of sheet before populating and eventually deleting
</commit_message>
<xml_diff>
--- a/Automated House Leads.xlsx
+++ b/Automated House Leads.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,9 +13,10 @@
     <sheet name="99AcresFilters" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="NoBrokerFilters" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="MagicBricksFilters" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="99Acres" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="NoBroker" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="MagicBricks" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="CommonFloor" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="99Acres" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="NoBroker" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="MagicBricks" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="117">
   <si>
     <t xml:space="preserve">Theory</t>
   </si>
@@ -203,6 +204,15 @@
   </si>
   <si>
     <t xml:space="preserve">Furnishedstatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact_person_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">furnish_state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fully</t>
   </si>
   <si>
     <t xml:space="preserve">Address</t>
@@ -532,7 +542,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="14.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -657,7 +667,7 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -666,7 +676,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="112.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="41.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="14.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -755,7 +765,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -862,7 +872,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -930,7 +940,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1009,65 +1019,84 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>66</v>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1077,92 +1106,56 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1181,6 +1174,110 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:Y1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.88"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AJ1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -1189,117 +1286,117 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>52</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>56</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="T1" s="3" t="s">
         <v>54</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="Y1" s="3" t="s">
         <v>33</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="AF1" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AG1" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AH1" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AI1" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AJ1" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>